<commit_message>
relecture carte et suivi
</commit_message>
<xml_diff>
--- a/EL_Electrical/Dashboard controller/Suivi_Dashboard Controller.xlsx
+++ b/EL_Electrical/Dashboard controller/Suivi_Dashboard Controller.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="742" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="742" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Généralités" sheetId="8" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
   <si>
     <r>
       <t>Identification de la carte :</t>
@@ -148,34 +148,13 @@
     <t>L'objectif est de la placer juste derrière le tableau de bord.</t>
   </si>
   <si>
-    <t>CAN0</t>
-  </si>
-  <si>
     <t>Entrées - Sortie de Dashboard Controller :</t>
   </si>
   <si>
-    <t>CAN0_INT</t>
-  </si>
-  <si>
     <t>shield can</t>
   </si>
   <si>
-    <t>LC_LED_PIN</t>
-  </si>
-  <si>
     <t>led launch control</t>
-  </si>
-  <si>
-    <t>SL_PIN</t>
-  </si>
-  <si>
-    <t>H_PIN</t>
-  </si>
-  <si>
-    <t>N_PIN</t>
-  </si>
-  <si>
-    <t>SC_PIN</t>
   </si>
   <si>
     <t>Serial TTL, écran</t>
@@ -223,18 +202,12 @@
     <t xml:space="preserve">Commentaire </t>
   </si>
   <si>
-    <t>5V (mais modifiable)</t>
-  </si>
-  <si>
     <t>12V</t>
   </si>
   <si>
     <t>Bouton launch control</t>
   </si>
   <si>
-    <t>5V ou 3,3V</t>
-  </si>
-  <si>
     <t>shift led bleu</t>
   </si>
   <si>
@@ -265,9 +238,6 @@
     <t>LC_BUTTON</t>
   </si>
   <si>
-    <t>LC_BUTTON_PIN</t>
-  </si>
-  <si>
     <t>5V ou 12V</t>
   </si>
   <si>
@@ -280,9 +250,6 @@
     <t>Log_SWITCH_PIN</t>
   </si>
   <si>
-    <t>digital</t>
-  </si>
-  <si>
     <t>bouton puis vers CAN</t>
   </si>
   <si>
@@ -326,6 +293,33 @@
   </si>
   <si>
     <t>Log_SWITCH</t>
+  </si>
+  <si>
+    <t>SC2 3,3V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SC1 3,3V</t>
+  </si>
+  <si>
+    <t>NEUTRE_BUTTON</t>
+  </si>
+  <si>
+    <t>HOMING_BUTTON</t>
+  </si>
+  <si>
+    <t>SL_BLUE_PIN</t>
+  </si>
+  <si>
+    <t>SL_RED_PIN</t>
+  </si>
+  <si>
+    <t>CAN-TX_HARDWARE</t>
+  </si>
+  <si>
+    <t>CAN-RX_HARDWARE</t>
+  </si>
+  <si>
+    <t>Bus CAN</t>
   </si>
 </sst>
 </file>
@@ -749,6 +743,52 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -761,21 +801,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -790,42 +817,54 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -834,51 +873,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -974,7 +968,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91CF59D6-7643-48F1-9CE0-9F4094EA5781}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91CF59D6-7643-48F1-9CE0-9F4094EA5781}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1040,7 +1034,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0CAA4BE7-D97B-4002-A238-954BD0BCACC4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CAA4BE7-D97B-4002-A238-954BD0BCACC4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1106,7 +1100,7 @@
         <xdr:cNvPr id="4" name="Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{87EA9B2B-AE46-40CF-8E98-D77E47E45061}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87EA9B2B-AE46-40CF-8E98-D77E47E45061}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1172,7 +1166,7 @@
         <xdr:cNvPr id="5" name="Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38013F2D-A221-4D0D-99E4-EBE76BB06D40}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38013F2D-A221-4D0D-99E4-EBE76BB06D40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1238,7 +1232,7 @@
         <xdr:cNvPr id="6" name="Rectangle 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9ECF62F8-D56F-45EF-AEC6-B04F2E1B33A4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ECF62F8-D56F-45EF-AEC6-B04F2E1B33A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1304,7 +1298,7 @@
         <xdr:cNvPr id="7" name="Rectangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F04B981-A14D-4442-982B-C915CAD2A250}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F04B981-A14D-4442-982B-C915CAD2A250}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1370,7 +1364,7 @@
         <xdr:cNvPr id="8" name="Rectangle 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{118586FF-7362-4E12-9EE2-1F6DB5D14E19}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{118586FF-7362-4E12-9EE2-1F6DB5D14E19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1436,7 +1430,7 @@
         <xdr:cNvPr id="9" name="Rectangle 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4349179F-DF46-4A41-B6FC-BAE8DDF8E4C9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4349179F-DF46-4A41-B6FC-BAE8DDF8E4C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1792,65 +1786,65 @@
       <c r="A1" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="21">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="52" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="51" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="14"/>
@@ -1862,179 +1856,163 @@
       <c r="H13" s="11"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="52" t="s">
+      <c r="B20" s="63"/>
+      <c r="C20" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="55"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="13"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="48"/>
+      <c r="B33" s="64"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="B34" s="52" t="s">
+      <c r="B34" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="F34" s="54" t="s">
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="F34" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="F35" s="54" t="s">
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="F35" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="F36" s="54" t="s">
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="F36" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="F37" s="54" t="s">
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="F37" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B34:D34"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
@@ -2051,6 +2029,22 @@
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C27:H28"/>
     <mergeCell ref="C16:H16"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C20:G20"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2070,7 +2064,7 @@
   </sheetPr>
   <dimension ref="A2:P46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:F9"/>
     </sheetView>
   </sheetViews>
@@ -2091,8 +2085,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.6" customHeight="1">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
@@ -2100,8 +2094,8 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="15.6">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="71"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="19"/>
@@ -2114,9 +2108,9 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.6" customHeight="1">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
+      <c r="A4" s="73"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
       <c r="F4" s="17"/>
@@ -2127,8 +2121,8 @@
       <c r="N4" s="24"/>
     </row>
     <row r="5" spans="1:16" ht="15.6" customHeight="1">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="18"/>
@@ -2140,14 +2134,14 @@
       <c r="N5" s="24"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
+      <c r="A6" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
       <c r="H6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="24"/>
@@ -2155,32 +2149,32 @@
       <c r="N6" s="24"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="61"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
       <c r="H7" s="6"/>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="61"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
       <c r="H8" s="6"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:16" ht="81.75" customHeight="1">
-      <c r="A9" s="61"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:16">
@@ -2189,20 +2183,20 @@
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:16" ht="55.8" customHeight="1">
-      <c r="A11" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
+      <c r="A11" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="56"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
       <c r="E12" s="6"/>
       <c r="G12" s="3"/>
       <c r="H12" s="6"/>
@@ -2213,55 +2207,55 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17" s="57"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
     </row>
     <row r="18" spans="1:8" ht="44.25" customHeight="1">
-      <c r="A18" s="57"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
     </row>
     <row r="19" spans="1:8">
       <c r="B19" s="6"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
+      <c r="A20" s="74"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:8">
@@ -2269,58 +2263,58 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
-      <c r="A22" s="57"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
+      <c r="A22" s="75"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
     </row>
     <row r="23" spans="1:8" ht="13.8">
-      <c r="A23" s="57"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
+      <c r="A23" s="75"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="57"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="57"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
+      <c r="A27" s="75"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="56"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:8">
@@ -2328,28 +2322,28 @@
       <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30" s="57"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
+      <c r="A30" s="75"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
     </row>
     <row r="31" spans="1:8" ht="13.8">
-      <c r="A31" s="57"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
+      <c r="A31" s="75"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1">
-      <c r="A32" s="57"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
+      <c r="A32" s="75"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:6">
@@ -2367,44 +2361,44 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
-      <c r="A36" s="57"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
+      <c r="A36" s="75"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
-      <c r="A37" s="57"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
+      <c r="A37" s="75"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
     </row>
     <row r="38" spans="1:6" ht="13.8">
-      <c r="A38" s="57"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
+      <c r="A38" s="75"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
     </row>
     <row r="39" spans="1:6" ht="13.8">
-      <c r="A39" s="57"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
+      <c r="A39" s="75"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
-      <c r="A40" s="57"/>
-      <c r="B40" s="57"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="57"/>
+      <c r="A40" s="75"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="75"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
     </row>
     <row r="41" spans="1:6">
       <c r="B41" s="6"/>
@@ -2432,12 +2426,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:F9"/>
-    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A30:F32"/>
     <mergeCell ref="A36:F40"/>
@@ -2445,6 +2433,12 @@
     <mergeCell ref="A14:F18"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A22:F27"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:F9"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.38825757575757575" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2463,8 +2457,8 @@
   </sheetPr>
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A10" zoomScale="90" zoomScaleNormal="115" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="90" zoomScaleNormal="115" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -2482,20 +2476,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.45" customHeight="1">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="A1" s="89"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
       <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:15" ht="15">
-      <c r="A2" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
+      <c r="A2" s="85" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="10"/>
       <c r="E2" s="9"/>
       <c r="O2" s="10"/>
@@ -2506,10 +2500,10 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:15" ht="44.4" customHeight="1" thickBot="1">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="69"/>
+      <c r="B4" s="83"/>
       <c r="C4" s="40" t="s">
         <v>19</v>
       </c>
@@ -2523,250 +2517,250 @@
         <v>22</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H4" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="79" t="s">
-        <v>59</v>
+      <c r="I4" s="49" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1">
-      <c r="A5" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="83" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="81"/>
+      <c r="A5" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="84"/>
+      <c r="C5" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="51"/>
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
       <c r="G5" s="44" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H5" s="39"/>
-      <c r="I5" s="81" t="s">
-        <v>41</v>
+      <c r="I5" s="51" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1">
-      <c r="A6" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="83" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="81"/>
+      <c r="A6" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="84"/>
+      <c r="C6" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="51"/>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
       <c r="G6" s="43" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H6" s="27"/>
-      <c r="I6" s="81" t="s">
-        <v>62</v>
+      <c r="I6" s="51" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="28.8">
-      <c r="A7" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="91" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="82"/>
+      <c r="A7" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="87"/>
+      <c r="C7" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="52"/>
       <c r="E7" s="45"/>
       <c r="F7" s="45"/>
       <c r="G7" s="45" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="H7" s="45"/>
-      <c r="I7" s="92" t="s">
-        <v>85</v>
+      <c r="I7" s="60" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="83" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="81"/>
+      <c r="A8" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="87"/>
+      <c r="C8" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="51"/>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
       <c r="G8" s="43" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="H8" s="27"/>
-      <c r="I8" s="78" t="s">
-        <v>64</v>
+      <c r="I8" s="48" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="84" t="s">
-        <v>65</v>
+      <c r="A9" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="88"/>
+      <c r="C9" s="54" t="s">
+        <v>56</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
       <c r="G9" s="43" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H9" s="27"/>
-      <c r="I9" s="78" t="s">
-        <v>67</v>
+      <c r="I9" s="48" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="18.45" customHeight="1">
-      <c r="A10" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="84" t="s">
-        <v>65</v>
+      <c r="A10" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="88"/>
+      <c r="C10" s="54" t="s">
+        <v>56</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
       <c r="G10" s="43" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H10" s="27"/>
-      <c r="I10" s="78" t="s">
-        <v>67</v>
+      <c r="I10" s="48" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="18.45" customHeight="1">
-      <c r="A11" s="63" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="84" t="s">
-        <v>87</v>
+      <c r="A11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="84"/>
+      <c r="C11" s="54" t="s">
+        <v>76</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
       <c r="G11" s="43" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H11" s="27"/>
-      <c r="I11" s="78" t="s">
+      <c r="I11" s="48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="21" customHeight="1">
+      <c r="A12" s="84" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="84"/>
+      <c r="C12" s="54" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="21" customHeight="1">
-      <c r="A12" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="84" t="s">
-        <v>87</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
       <c r="G12" s="43" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H12" s="27"/>
-      <c r="I12" s="78" t="s">
-        <v>77</v>
+      <c r="I12" s="48" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="84" t="s">
-        <v>87</v>
+      <c r="A13" s="78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="79"/>
+      <c r="C13" s="54" t="s">
+        <v>76</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
       <c r="G13" s="43" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H13" s="27"/>
-      <c r="I13" s="78" t="s">
-        <v>92</v>
+      <c r="I13" s="48" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="14.4" customHeight="1">
-      <c r="A14" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="84" t="s">
-        <v>87</v>
+      <c r="A14" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="87"/>
+      <c r="C14" s="54" t="s">
+        <v>76</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
       <c r="G14" s="45" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H14" s="28"/>
-      <c r="I14" s="78" t="s">
-        <v>93</v>
+      <c r="I14" s="48" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="18.45" customHeight="1">
-      <c r="A15" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="81" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="85"/>
+      <c r="A15" s="84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="84"/>
+      <c r="C15" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="55"/>
       <c r="G15" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81" t="s">
-        <v>83</v>
+        <v>65</v>
+      </c>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="64"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="84"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
       <c r="G16" s="43"/>
       <c r="H16" s="27"/>
-      <c r="I16" s="78"/>
+      <c r="I16" s="48"/>
     </row>
     <row r="17" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A17" s="64"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="84"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
       <c r="G17" s="43"/>
       <c r="H17" s="27"/>
-      <c r="I17" s="78"/>
+      <c r="I17" s="48"/>
     </row>
     <row r="18" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A18" s="64"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="84"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="27"/>
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
@@ -2775,9 +2769,9 @@
       <c r="I18" s="25"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="64"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="84"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="54"/>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
@@ -2786,9 +2780,9 @@
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A20" s="64"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="84"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="54"/>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
@@ -2797,9 +2791,9 @@
       <c r="I20" s="25"/>
     </row>
     <row r="21" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A21" s="64"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="84"/>
+      <c r="A21" s="78"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="54"/>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
@@ -2808,9 +2802,9 @@
       <c r="I21" s="25"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="64"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="84"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="54"/>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
@@ -2824,270 +2818,276 @@
       <c r="I23" s="26"/>
     </row>
     <row r="24" spans="1:9" ht="18.45" customHeight="1" thickBot="1">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="29"/>
       <c r="I24" s="26"/>
     </row>
     <row r="25" spans="1:9" ht="18.45" customHeight="1" thickBot="1">
-      <c r="A25" s="88" t="s">
+      <c r="A25" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="89"/>
-      <c r="C25" s="68" t="s">
+      <c r="B25" s="77"/>
+      <c r="C25" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="68" t="s">
+      <c r="D25" s="83"/>
+      <c r="E25" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="69"/>
+      <c r="F25" s="83"/>
       <c r="G25" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="79" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="H25" s="49" t="s">
+        <v>52</v>
       </c>
       <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" thickBot="1">
-      <c r="A26" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="74"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="H26" s="86" t="s">
+      <c r="A26" s="80" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="81"/>
+      <c r="C26" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="81"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="25"/>
+    </row>
+    <row r="27" spans="1:9" ht="18.45" customHeight="1">
+      <c r="A27" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="79"/>
+      <c r="C27" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="79"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="25"/>
+    </row>
+    <row r="28" spans="1:9" ht="18.45" customHeight="1">
+      <c r="A28" s="78" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="79"/>
+      <c r="C28" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="79"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" s="25"/>
+    </row>
+    <row r="29" spans="1:9" ht="18.45" customHeight="1">
+      <c r="A29" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="79"/>
+      <c r="C29" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="79"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" s="25"/>
+    </row>
+    <row r="30" spans="1:9" ht="18.45" customHeight="1">
+      <c r="A30" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="79"/>
+      <c r="C30" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="79"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="43">
+        <v>0</v>
+      </c>
+      <c r="H30" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30" s="25"/>
+    </row>
+    <row r="31" spans="1:9" ht="18.45" customHeight="1">
+      <c r="A31" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="79"/>
+      <c r="C31" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="79"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="43">
+        <v>0</v>
+      </c>
+      <c r="H31" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" s="25"/>
+    </row>
+    <row r="32" spans="1:9" ht="18.45" customHeight="1">
+      <c r="A32" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="79"/>
+      <c r="C32" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="79"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="43">
+        <v>0</v>
+      </c>
+      <c r="H32" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="I32" s="25"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="87"/>
+      <c r="C33" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="79"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="43">
+        <v>0</v>
+      </c>
+      <c r="H33" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="86" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="87"/>
+      <c r="C34" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="79"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="43">
+        <v>0</v>
+      </c>
+      <c r="H34" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="I34" s="25"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="86" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="87"/>
+      <c r="C35" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="79"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="43">
+        <v>0</v>
+      </c>
+      <c r="H35" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="I26" s="25"/>
-    </row>
-    <row r="27" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A27" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="H27" s="87" t="s">
-        <v>39</v>
-      </c>
-      <c r="I27" s="25"/>
-    </row>
-    <row r="28" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A28" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="65"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="I28" s="25"/>
-    </row>
-    <row r="29" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A29" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="65"/>
-      <c r="C29" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="65"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="I29" s="25"/>
-    </row>
-    <row r="30" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A30" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="64" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="65"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="I30" s="25"/>
-    </row>
-    <row r="31" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A31" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="65"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="I31" s="25"/>
-    </row>
-    <row r="32" spans="1:9" ht="18.45" customHeight="1">
-      <c r="A32" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="65"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="H32" s="81" t="s">
-        <v>51</v>
-      </c>
-      <c r="I32" s="25"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="65"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="I33" s="25"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="71"/>
-      <c r="C34" s="64" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="65"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="81" t="s">
+      <c r="I35" s="25"/>
+    </row>
+    <row r="36" spans="1:9" ht="14.4" customHeight="1">
+      <c r="A36" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="79"/>
+      <c r="C36" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="79"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="I34" s="25"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="71"/>
-      <c r="C35" s="64" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="65"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="81" t="s">
-        <v>46</v>
-      </c>
-      <c r="I35" s="25"/>
-    </row>
-    <row r="36" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A36" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="65"/>
-      <c r="C36" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="65"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="81" t="s">
-        <v>54</v>
-      </c>
       <c r="I36" s="25"/>
     </row>
     <row r="37" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A37" s="64" t="s">
+      <c r="A37" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="79"/>
+      <c r="C37" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="79"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="65"/>
-      <c r="C37" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="65"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="81" t="s">
-        <v>55</v>
+      <c r="H37" s="51" t="s">
+        <v>48</v>
       </c>
       <c r="I37" s="25"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="64"/>
+      <c r="A38" s="84"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="84"/>
+      <c r="F38" s="78"/>
       <c r="G38" s="43"/>
-      <c r="H38" s="81" t="s">
-        <v>83</v>
+      <c r="H38" s="51" t="s">
+        <v>72</v>
       </c>
       <c r="I38" s="25"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="90"/>
-      <c r="B39" s="90"/>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="90"/>
-      <c r="F39" s="90"/>
-      <c r="G39" s="90"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
     </row>
@@ -3134,20 +3134,32 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="E36:F36"/>
@@ -3164,41 +3176,29 @@
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3760,451 +3760,449 @@
       <c r="A1" s="15"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="76"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
+      <c r="A4" s="90"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
     </row>
     <row r="5" spans="1:7" ht="13.65" customHeight="1">
-      <c r="A5" s="76"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="76"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A8" s="75"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
+      <c r="A8" s="90"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
     </row>
     <row r="9" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A9" s="75"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
     </row>
     <row r="10" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
+      <c r="A10" s="90"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
     </row>
     <row r="11" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
     </row>
     <row r="12" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A12" s="75"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="75"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
+      <c r="A13" s="90"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="75"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
+      <c r="A14" s="90"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="75"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="75"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
+      <c r="A16" s="90"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="75"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="75"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
+      <c r="A18" s="90"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="75"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
+      <c r="A19" s="90"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="75"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
+      <c r="A20" s="90"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="75"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
+      <c r="A21" s="90"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="75"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
+      <c r="A22" s="90"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="75"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
+      <c r="A23" s="90"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="75"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
+      <c r="A24" s="90"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="90"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
+      <c r="A25" s="90"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="75"/>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
+      <c r="A26" s="90"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="75"/>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
+      <c r="A27" s="90"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="75"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
+      <c r="A28" s="90"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="75"/>
-      <c r="B29" s="75"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
+      <c r="A29" s="90"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="75"/>
-      <c r="B30" s="75"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
+      <c r="A30" s="90"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="75"/>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="90"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="75"/>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="75"/>
+      <c r="A32" s="90"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="90"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="75"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
+      <c r="A33" s="90"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="75"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
+      <c r="A34" s="90"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="75"/>
-      <c r="B35" s="75"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="75"/>
-      <c r="B36" s="75"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="75"/>
+      <c r="A36" s="90"/>
+      <c r="B36" s="90"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="90"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="75"/>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
+      <c r="A37" s="90"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="90"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="75"/>
-      <c r="B38" s="75"/>
-      <c r="C38" s="75"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
+      <c r="A38" s="90"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="90"/>
+      <c r="D38" s="90"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="90"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="75"/>
-      <c r="B39" s="75"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="75"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
+      <c r="A39" s="90"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="90"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="90"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="75"/>
-      <c r="B40" s="75"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
+      <c r="A40" s="90"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="90"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="90"/>
+      <c r="G40" s="90"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="75"/>
-      <c r="B41" s="75"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
+      <c r="A41" s="90"/>
+      <c r="B41" s="90"/>
+      <c r="C41" s="90"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="90"/>
+      <c r="G41" s="90"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="75"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="75"/>
+      <c r="A42" s="90"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="90"/>
+      <c r="D42" s="90"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="90"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="75"/>
-      <c r="B43" s="75"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="75"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="75"/>
+      <c r="A43" s="90"/>
+      <c r="B43" s="90"/>
+      <c r="C43" s="90"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="90"/>
+      <c r="F43" s="90"/>
+      <c r="G43" s="90"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="75"/>
-      <c r="B44" s="75"/>
-      <c r="C44" s="75"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="75"/>
+      <c r="A44" s="90"/>
+      <c r="B44" s="90"/>
+      <c r="C44" s="90"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="90"/>
+      <c r="G44" s="90"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="75"/>
-      <c r="B45" s="75"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="75"/>
+      <c r="A45" s="90"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="90"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="75"/>
-      <c r="B46" s="75"/>
-      <c r="C46" s="75"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="75"/>
+      <c r="A46" s="90"/>
+      <c r="B46" s="90"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="90"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="75"/>
-      <c r="B47" s="75"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
+      <c r="A47" s="90"/>
+      <c r="B47" s="90"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="90"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="90"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="75"/>
-      <c r="B48" s="75"/>
-      <c r="C48" s="75"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="75"/>
-      <c r="G48" s="75"/>
+      <c r="A48" s="90"/>
+      <c r="B48" s="90"/>
+      <c r="C48" s="90"/>
+      <c r="D48" s="90"/>
+      <c r="E48" s="90"/>
+      <c r="F48" s="90"/>
+      <c r="G48" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F43:G43"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A48:B48"/>
@@ -4221,34 +4219,36 @@
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:E38"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:G30"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>